<commit_message>
Used a new model to compute yo2y
</commit_message>
<xml_diff>
--- a/Data/quarter_on_quarter_Q1_2020.xlsx
+++ b/Data/quarter_on_quarter_Q1_2020.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
-    <t>Tracker (yo2y)</t>
+    <t>Tracker (yoy)</t>
   </si>
   <si>
     <t>region</t>
@@ -531,7 +531,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3.4875412212938</v>
+        <v>3.997431822067821</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -539,7 +539,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2.650943688167895</v>
+        <v>3.507738076960831</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -547,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.02459203582712011</v>
+        <v>-0.6219318845783861</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -555,7 +555,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.6157508186148908</v>
+        <v>1.35041188314875</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -563,7 +563,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>-0.7068263605403913</v>
+        <v>0.5494206840561455</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -571,7 +571,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>4.992969857022422</v>
+        <v>5.154642321020941</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -579,7 +579,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.02470967057386364</v>
+        <v>0.5513447351755074</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -587,7 +587,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>-2.003749902842278</v>
+        <v>-2.422392786878991</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -595,7 +595,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>-0.28858885970382</v>
+        <v>0.8459790876528261</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -603,7 +603,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>-0.7135308184723743</v>
+        <v>0.1157408238356528</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1.02392067392465</v>
+        <v>3.540058817858083</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -619,7 +619,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>1.701290420850099</v>
+        <v>3.548719203771689</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -627,7 +627,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.08339145197036046</v>
+        <v>1.677649134169701</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -635,7 +635,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.5236533163672119</v>
+        <v>0.728128150653462</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -643,7 +643,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>-1.393378281211477</v>
+        <v>-1.284171144984669</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -651,7 +651,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.4376343062808319</v>
+        <v>0.6465608374731646</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -659,7 +659,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>2.375856715924862</v>
+        <v>4.028908876135762</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -667,7 +667,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>2.311618696074813</v>
+        <v>-0.8853013920439023</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -675,7 +675,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>4.132188280572735</v>
+        <v>3.043700757466139</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -683,7 +683,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>2.565314150723585</v>
+        <v>1.792946972473097</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -691,7 +691,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>-1.939804459840233</v>
+        <v>-1.330779030561458</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -699,7 +699,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>2.694525259382097</v>
+        <v>4.293095544127379</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -707,7 +707,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.353157960824535</v>
+        <v>0.5271650709245401</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -715,7 +715,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>-0.6996086634524779</v>
+        <v>1.207794540244223</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -723,7 +723,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>1.171515630939712</v>
+        <v>0.6875775215922753</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -731,7 +731,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.7300892801959113</v>
+        <v>2.053657220440286</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -739,7 +739,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>1.507100356252189</v>
+        <v>1.385049210071831</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -747,7 +747,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>1.602961389154522</v>
+        <v>2.267413823955633</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -755,7 +755,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>1.414735600758443</v>
+        <v>2.181221137737266</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -763,7 +763,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.2200253414871511</v>
+        <v>0.5340766838090261</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -771,7 +771,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>1.448112597112328</v>
+        <v>2.561469987863085</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -779,7 +779,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>-0.9747564697741296</v>
+        <v>-0.8434777660186188</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -787,7 +787,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>2.080118480591686</v>
+        <v>2.742529675130223</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -795,7 +795,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>-1.850745070803272</v>
+        <v>-0.9456210172690382</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -803,7 +803,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>3.004267259425619</v>
+        <v>3.175229136339963</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -811,7 +811,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>3.218469440645011</v>
+        <v>2.280434039863155</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -819,7 +819,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>-3.778863960978829</v>
+        <v>-3.537696405876434</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -827,7 +827,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>1.514329140180681</v>
+        <v>1.864974102403472</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -835,7 +835,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>-2.489226735803318</v>
+        <v>-2.600824064847018</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -843,7 +843,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>0.7757704840517077</v>
+        <v>1.739708944864859</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -851,7 +851,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.6722696706463971</v>
+        <v>1.109473804490002</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -859,7 +859,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>-0.1569159323475566</v>
+        <v>-0.1696800102653051</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -867,7 +867,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0.6959208425978192</v>
+        <v>-0.05158516532106638</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -875,7 +875,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>-1.352248009645352</v>
+        <v>-0.7357271084382444</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -883,7 +883,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>1.363725294608198</v>
+        <v>1.429893097472057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>